<commit_message>
updated readme and excel
</commit_message>
<xml_diff>
--- a/thoughts.xlsx
+++ b/thoughts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t xml:space="preserve">What is EDM?</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Elelectronic Dance Music.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
   <si>
     <t xml:space="preserve">Its main characteristic, however, is that it is mainly electronic. Do keep in mind though,</t>
@@ -278,13 +281,13 @@
   <dimension ref="A4:F47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.0561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,28 +306,29 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -337,7 +341,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -345,7 +349,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -353,32 +357,32 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="7" t="n">
         <v>0.2</v>
@@ -386,7 +390,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7" t="n">
         <v>0.2</v>
@@ -394,7 +398,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="7" t="n">
         <v>0.15</v>
@@ -402,7 +406,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" s="7" t="n">
         <v>0.05</v>
@@ -410,7 +414,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7" t="n">
         <v>0.1</v>
@@ -418,7 +422,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="7" t="n">
         <v>0.05</v>
@@ -426,7 +430,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="7" t="n">
         <v>0.15</v>
@@ -434,22 +438,22 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -457,87 +461,87 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>